<commit_message>
Update the test files to include cross diagonal borders.
</commit_message>
<xml_diff>
--- a/test/xlsx/borders/directions.xlsx
+++ b/test/xlsx/borders/directions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kohei\workspace\orcus\test\xlsx\borders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\workspace\orcus\test\xlsx\borders\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>top</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>tr to bl</t>
+  </si>
+  <si>
+    <t>cross diagonal</t>
   </si>
 </sst>
 </file>
@@ -65,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -119,6 +122,15 @@
       </diagonal>
     </border>
     <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
       <left/>
       <right/>
       <top/>
@@ -131,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -139,6 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,9 +466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498368F4-78A1-4F71-BA2B-E5F1F20CC342}">
-  <dimension ref="B2:B12"/>
+  <dimension ref="B2:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -492,7 +507,13 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>